<commit_message>
add traffic data pictures, fix organization issues in chapter 2
</commit_message>
<xml_diff>
--- a/data/raw_traffic/alldata.xlsx
+++ b/data/raw_traffic/alldata.xlsx
@@ -4,7 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="0" windowWidth="25040" windowHeight="16980" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="720" yWindow="0" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bytes" sheetId="1" r:id="rId1"/>
@@ -172,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="3">
   <si>
     <t>Interval start</t>
   </si>
@@ -180,28 +181,7 @@
     <t>AirPlay</t>
   </si>
   <si>
-    <t>AirPlay 500k</t>
-  </si>
-  <si>
-    <t>AirPlay 700k</t>
-  </si>
-  <si>
-    <t>AirPlay 1000k</t>
-  </si>
-  <si>
     <t>DLNA</t>
-  </si>
-  <si>
-    <t>DLNA 500k</t>
-  </si>
-  <si>
-    <t>DLNA 700k</t>
-  </si>
-  <si>
-    <t>DLNA 1000k</t>
-  </si>
-  <si>
-    <t>AirPadslay</t>
   </si>
 </sst>
 </file>
@@ -2332,20 +2312,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2126894728"/>
-        <c:axId val="2088501960"/>
+        <c:axId val="-2070664264"/>
+        <c:axId val="-2070661288"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2126894728"/>
+        <c:axId val="-2070664264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088501960"/>
+        <c:crossAx val="-2070661288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2353,18 +2352,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2088501960"/>
+        <c:axId val="-2070661288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126894728"/>
+        <c:crossAx val="-2070664264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2415,7 +2438,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 500k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3460,7 +3483,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 500k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4482,20 +4505,44 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2107335192"/>
-        <c:axId val="-2107332568"/>
+        <c:axId val="-2070631160"/>
+        <c:axId val="-2070628184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2107335192"/>
+        <c:axId val="-2070631160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107332568"/>
+        <c:crossAx val="-2070628184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4503,18 +4550,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107332568"/>
+        <c:axId val="-2070628184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (bytes)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2107335192"/>
+        <c:crossAx val="-2070631160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4565,7 +4636,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 700k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5583,7 +5654,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 700k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6617,20 +6688,44 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108614696"/>
-        <c:axId val="-2108352024"/>
+        <c:axId val="-2070601688"/>
+        <c:axId val="-2070598712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108614696"/>
+        <c:axId val="-2070601688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108352024"/>
+        <c:crossAx val="-2070598712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6638,18 +6733,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108352024"/>
+        <c:axId val="-2070598712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108614696"/>
+        <c:crossAx val="-2070601688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6700,7 +6814,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 1000k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7733,7 +7847,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 1000k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8758,20 +8872,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2080075560"/>
-        <c:axId val="-2110803144"/>
+        <c:axId val="-2070571688"/>
+        <c:axId val="-2070568712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2080075560"/>
+        <c:axId val="-2070571688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110803144"/>
+        <c:crossAx val="-2070568712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8779,18 +8912,42 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110803144"/>
+        <c:axId val="-2070568712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (packets)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080075560"/>
+        <c:crossAx val="-2070571688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8841,7 +8998,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPadslay</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -10896,20 +11053,44 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2105842920"/>
-        <c:axId val="-2105839944"/>
+        <c:axId val="2088494952"/>
+        <c:axId val="-2112138776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2105842920"/>
+        <c:axId val="2088494952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105839944"/>
+        <c:crossAx val="-2112138776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10917,18 +11098,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105839944"/>
+        <c:axId val="-2112138776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic (packets)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105842920"/>
+        <c:crossAx val="2088494952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10979,7 +11179,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 500k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -12024,7 +12224,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 500k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -13046,20 +13246,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2073339960"/>
-        <c:axId val="-2073336984"/>
+        <c:axId val="-2108802440"/>
+        <c:axId val="2123621928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2073339960"/>
+        <c:axId val="-2108802440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073336984"/>
+        <c:crossAx val="2123621928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13067,18 +13286,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2073336984"/>
+        <c:axId val="2123621928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic (packets)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2073339960"/>
+        <c:crossAx val="-2108802440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13129,7 +13367,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 700k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -14147,7 +14385,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 700k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -15181,20 +15419,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2077182536"/>
-        <c:axId val="-2079213784"/>
+        <c:axId val="-2112832184"/>
+        <c:axId val="-2112487528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2077182536"/>
+        <c:axId val="-2112832184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2079213784"/>
+        <c:crossAx val="-2112487528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15202,18 +15459,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079213784"/>
+        <c:axId val="-2112487528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic (packets)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077182536"/>
+        <c:crossAx val="-2112832184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15264,7 +15540,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AirPlay 1000k</c:v>
+                  <c:v>AirPlay</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -16297,7 +16573,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>DLNA 1000k</c:v>
+                  <c:v>DLNA</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -17322,20 +17598,39 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2105814264"/>
-        <c:axId val="-2105811288"/>
+        <c:axId val="-2109201624"/>
+        <c:axId val="-2112151672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2105814264"/>
+        <c:axId val="-2109201624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105811288"/>
+        <c:crossAx val="-2112151672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17343,18 +17638,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2105811288"/>
+        <c:axId val="-2112151672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Traffic (packets)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105814264"/>
+        <c:crossAx val="-2109201624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -17380,16 +17694,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17417,9 +17731,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>67</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17446,10 +17760,10 @@
       <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>89</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17471,15 +17785,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>635000</xdr:colOff>
-      <xdr:row>109</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17512,9 +17826,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17544,9 +17858,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17576,9 +17890,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>546100</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17601,16 +17915,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>75</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
-      <xdr:row>92</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17639,15 +17953,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_700k" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_500k" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_500k" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_700k" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17655,27 +17969,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_700k" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_500k" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_500k" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_700k" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_700k" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_500k" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_500k" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_700k" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17683,15 +17997,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_700k" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_500k" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_500k" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_700k" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18022,8 +18336,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J340"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="1">
+      <selection activeCell="T118" sqref="T118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -18045,25 +18362,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -27752,9 +28069,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -27765,8 +28084,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J340"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A54" workbookViewId="0">
       <selection activeCell="M64" sqref="M64"/>
+    </sheetView>
+    <sheetView topLeftCell="A59" workbookViewId="1">
+      <selection activeCell="V85" sqref="V85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -27782,28 +28104,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -37496,6 +37818,7 @@
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
update figures, scale to 1000kb
</commit_message>
<xml_diff>
--- a/data/raw_traffic/alldata.xlsx
+++ b/data/raw_traffic/alldata.xlsx
@@ -4,8 +4,8 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="0" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28080" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="760" yWindow="0" windowWidth="25040" windowHeight="16980" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="0" windowWidth="25720" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bytes" sheetId="1" r:id="rId1"/>
@@ -2312,11 +2312,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2070664264"/>
-        <c:axId val="-2070661288"/>
+        <c:axId val="-2091226552"/>
+        <c:axId val="-2091219688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070664264"/>
+        <c:axId val="-2091226552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2344,7 +2344,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070661288"/>
+        <c:crossAx val="-2091219688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2352,7 +2352,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070661288"/>
+        <c:axId val="-2091219688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2374,7 +2374,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (bytes)</a:t>
+                  <a:t> (Kbytes)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -2387,9 +2387,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070664264"/>
+        <c:crossAx val="-2091226552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -4505,11 +4508,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2070631160"/>
-        <c:axId val="-2070628184"/>
+        <c:axId val="-2089982920"/>
+        <c:axId val="-2089977208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070631160"/>
+        <c:axId val="-2089982920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4542,7 +4545,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070628184"/>
+        <c:crossAx val="-2089977208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4550,7 +4553,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070628184"/>
+        <c:axId val="-2089977208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4572,7 +4575,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (bytes)</a:t>
+                  <a:t> (Kbytes)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -4585,9 +4588,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070631160"/>
+        <c:crossAx val="-2089982920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -6688,11 +6694,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2070601688"/>
-        <c:axId val="-2070598712"/>
+        <c:axId val="-2089947928"/>
+        <c:axId val="-2089942216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070601688"/>
+        <c:axId val="-2089947928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6725,7 +6731,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070598712"/>
+        <c:crossAx val="-2089942216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6733,7 +6739,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070598712"/>
+        <c:axId val="-2089942216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6751,7 +6757,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Traffic (bytes)</a:t>
+                  <a:t>Traffic (Kbytes)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6763,9 +6769,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070601688"/>
+        <c:crossAx val="-2089947928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -8872,11 +8881,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2070571688"/>
-        <c:axId val="-2070568712"/>
+        <c:axId val="-2089912696"/>
+        <c:axId val="-2089907224"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070571688"/>
+        <c:axId val="-2089912696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8904,7 +8913,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070568712"/>
+        <c:crossAx val="-2089907224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8912,7 +8921,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070568712"/>
+        <c:axId val="-2089907224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8934,7 +8943,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (packets)</a:t>
+                  <a:t> (Kbytes)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-US"/>
               </a:p>
@@ -8947,9 +8956,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2070571688"/>
+        <c:crossAx val="-2089912696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -11053,11 +11065,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2088494952"/>
-        <c:axId val="-2112138776"/>
+        <c:axId val="-2093024696"/>
+        <c:axId val="-2093018984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2088494952"/>
+        <c:axId val="-2093024696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11084,13 +11096,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112138776"/>
+        <c:crossAx val="-2093018984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11098,7 +11109,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112138776"/>
+        <c:axId val="-2093018984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11121,21 +11132,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2088494952"/>
+        <c:crossAx val="-2093024696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -13246,11 +13255,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2108802440"/>
-        <c:axId val="2123621928"/>
+        <c:axId val="-2092986168"/>
+        <c:axId val="-2092980712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2108802440"/>
+        <c:axId val="-2092986168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13272,13 +13281,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2123621928"/>
+        <c:crossAx val="-2092980712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13286,7 +13294,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2123621928"/>
+        <c:axId val="-2092980712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13309,21 +13317,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108802440"/>
+        <c:crossAx val="-2092986168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -15419,11 +15425,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2112832184"/>
-        <c:axId val="-2112487528"/>
+        <c:axId val="-2089788616"/>
+        <c:axId val="-2089783160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2112832184"/>
+        <c:axId val="-2089788616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15445,13 +15451,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112487528"/>
+        <c:crossAx val="-2089783160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -15459,7 +15464,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112487528"/>
+        <c:axId val="-2089783160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15482,21 +15487,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112832184"/>
+        <c:crossAx val="-2089788616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17598,11 +17601,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2109201624"/>
-        <c:axId val="-2112151672"/>
+        <c:axId val="-2089753080"/>
+        <c:axId val="-2089747624"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2109201624"/>
+        <c:axId val="-2089753080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17624,13 +17627,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112151672"/>
+        <c:crossAx val="-2089747624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -17638,7 +17640,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112151672"/>
+        <c:axId val="-2089747624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -17661,21 +17663,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109201624"/>
+        <c:crossAx val="-2089753080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -17953,15 +17953,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_700k" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_500k" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_500k" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_700k" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17969,27 +17969,27 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets" connectionId="16" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_700k" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_500k" connectionId="14" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets_bw_500k" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_packets_bw_700k" connectionId="15" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_packets" connectionId="8" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_700k" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_500k" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_500k" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_700k" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17997,15 +17997,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_700k" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_500k" connectionId="10" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes_bw_500k" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dlna_bytes_bw_700k" connectionId="11" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="airplay_bytes" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
@@ -18339,8 +18339,8 @@
     <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="1">
-      <selection activeCell="T118" sqref="T118"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="1">
+      <selection activeCell="O121" sqref="O121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>